<commit_message>
corrected typo c --> 16 in one cell
</commit_message>
<xml_diff>
--- a/data/specs_PLT2_rep3_on11thsept.xlsx
+++ b/data/specs_PLT2_rep3_on11thsept.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia_local\Dropbox\Olivia\Data analysis\growth rate assays 23 sept\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s4528540\Documents\exp-evol\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B494EAC-BC7A-485C-B84E-C3F37702F269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="128">
   <si>
     <t>Row</t>
   </si>
@@ -408,15 +409,12 @@
   </si>
   <si>
     <t>OH_AB13STP3</t>
-  </si>
-  <si>
-    <t>c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -734,11 +732,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5:R18"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1600,8 +1598,8 @@
       <c r="H27" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="I27" s="1" t="s">
-        <v>128</v>
+      <c r="I27" s="1">
+        <v>16</v>
       </c>
       <c r="J27" s="1">
         <v>0</v>

</xml_diff>